<commit_message>
Nya protokoll 1-3 star
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Showklass_Protokoll och resutatfil.xlsx
+++ b/mallar/Protokoll/Showklass_Protokoll och resutatfil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB83559B-524B-4872-A6DB-79A2DD05C6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BABA46A-D12B-4405-B268-D3EDED1C8714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="0" windowWidth="10800" windowHeight="12900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>1)</t>
   </si>
@@ -847,48 +847,6 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,17 +874,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -951,6 +948,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4772,13 +4772,13 @@
       <c r="Q13"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
       <c r="I14" s="32" t="s">
         <v>36</v>
       </c>
@@ -4799,17 +4799,17 @@
     </row>
     <row r="15" spans="1:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15"/>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="55" t="s">
+      <c r="C15" s="55"/>
+      <c r="D15" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
       <c r="K15" s="33"/>
@@ -4825,15 +4825,15 @@
     </row>
     <row r="16" spans="1:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="58" t="s">
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -4848,15 +4848,15 @@
       <c r="Q16"/>
     </row>
     <row r="17" spans="2:17" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="68"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="70" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -4871,17 +4871,17 @@
       <c r="Q17"/>
     </row>
     <row r="18" spans="2:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="55" t="s">
+      <c r="C18" s="55"/>
+      <c r="D18" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
       <c r="I18" s="33"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
@@ -4896,15 +4896,15 @@
       <c r="Q18"/>
     </row>
     <row r="19" spans="2:17" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="56" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
       <c r="I19" s="36"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
@@ -4919,17 +4919,17 @@
       <c r="Q19"/>
     </row>
     <row r="20" spans="2:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="57" t="s">
+      <c r="C20" s="68"/>
+      <c r="D20" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
       <c r="I20" s="37"/>
       <c r="J20" s="37"/>
       <c r="K20" s="37"/>
@@ -4944,15 +4944,15 @@
       <c r="Q20"/>
     </row>
     <row r="21" spans="2:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="58" t="s">
+      <c r="B21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
@@ -4967,15 +4967,15 @@
       <c r="Q21"/>
     </row>
     <row r="22" spans="2:17" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="58" t="s">
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
@@ -4990,15 +4990,15 @@
       <c r="Q22"/>
     </row>
     <row r="23" spans="2:17" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="56" t="s">
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
@@ -5087,17 +5087,17 @@
       <c r="Q27"/>
     </row>
     <row r="28" spans="2:17" ht="29.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="61"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="47"/>
       <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
@@ -5105,17 +5105,17 @@
       <c r="Q28"/>
     </row>
     <row r="29" spans="2:17" ht="27.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="64"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
@@ -5123,17 +5123,17 @@
       <c r="Q29"/>
     </row>
     <row r="30" spans="2:17" ht="23.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="65"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="67"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="53"/>
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
@@ -5324,11 +5324,6 @@
     <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B28:L30"/>
-    <mergeCell ref="B15:C17"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D17:H17"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B20:C23"/>
@@ -5338,6 +5333,11 @@
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="D23:H23"/>
+    <mergeCell ref="B28:L30"/>
+    <mergeCell ref="B15:C17"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5359,7 +5359,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -5408,11 +5408,11 @@
         <v>8</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="25"/>
       <c r="I4" s="28"/>
       <c r="J4" s="9" t="s">
@@ -5427,11 +5427,11 @@
         <v>9</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="I5" s="26"/>
       <c r="J5" s="9" t="s">
         <v>7</v>
@@ -5445,11 +5445,11 @@
         <v>16</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
       <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
@@ -5462,14 +5462,12 @@
         <v>10</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="I7" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
@@ -5482,14 +5480,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="I8" s="8" t="s">
-        <v>1</v>
-      </c>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -5499,32 +5495,36 @@
     </row>
     <row r="9" spans="1:15" ht="17.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H9"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
     </row>
     <row r="10" spans="1:15" ht="17.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10"/>
     </row>
     <row r="11" spans="1:15" ht="17.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11"/>
     </row>
     <row r="12" spans="1:15" ht="17.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
       <c r="M12"/>
     </row>
     <row r="13" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5535,10 +5535,10 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
       <c r="M13"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5546,13 +5546,13 @@
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:15" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="32" t="s">
         <v>36</v>
       </c>
@@ -5569,17 +5569,17 @@
     </row>
     <row r="16" spans="1:15" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16"/>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
       <c r="I16" s="33"/>
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
@@ -5591,15 +5591,15 @@
     </row>
     <row r="17" spans="1:13" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="58" t="s">
+      <c r="B17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -5610,15 +5610,15 @@
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13" ht="24.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="68"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="70" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -5629,17 +5629,17 @@
       <c r="M18"/>
     </row>
     <row r="19" spans="1:13" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="55" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
       <c r="I19" s="33"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
@@ -5650,15 +5650,15 @@
       <c r="M19"/>
     </row>
     <row r="20" spans="1:13" ht="24.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="56" t="s">
+      <c r="B20" s="65"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
@@ -5669,17 +5669,17 @@
       <c r="M20"/>
     </row>
     <row r="21" spans="1:13" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="57" t="s">
+      <c r="C21" s="68"/>
+      <c r="D21" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
       <c r="I21" s="37"/>
       <c r="J21" s="37"/>
       <c r="K21" s="37"/>
@@ -5690,15 +5690,15 @@
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="58" t="s">
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
@@ -5709,15 +5709,15 @@
       <c r="M22"/>
     </row>
     <row r="23" spans="1:13" ht="24.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="58" t="s">
+      <c r="B23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
@@ -5728,15 +5728,15 @@
       <c r="M23"/>
     </row>
     <row r="24" spans="1:13" ht="24.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="49"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="56" t="s">
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
@@ -5813,81 +5813,81 @@
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="76"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="75"/>
     </row>
     <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="79"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="78"/>
     </row>
     <row r="32" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="77"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="79"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="78"/>
     </row>
     <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="77"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="78"/>
-      <c r="L33" s="79"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="78"/>
     </row>
     <row r="34" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="77"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="79"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="78"/>
     </row>
     <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="80"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="71"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
       <c r="L35" s="81"/>
     </row>
     <row r="36" spans="2:13" ht="11.55" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5941,6 +5941,9 @@
     <row r="42" spans="2:13" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="B30:L35"/>
@@ -5957,9 +5960,6 @@
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="D24:H24"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="7.874015748031496E-2"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6101,15 +6101,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6175,6 +6166,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
   <ds:schemaRefs>
@@ -6191,14 +6191,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6213,4 +6205,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>